<commit_message>
fix more designer photo
</commit_message>
<xml_diff>
--- a/public/cardapiodata.xlsx
+++ b/public/cardapiodata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\mn-transparency\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB4A86C-CA67-4CB4-B110-39CD0AFF3628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3062E405-3830-4DB6-B77B-765B639B07BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{92F38698-8C92-4FAD-975C-8E92F285CBE1}"/>
   </bookViews>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2493752C-554F-479C-841E-F450C946588B}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mvp 01 uptade 1
</commit_message>
<xml_diff>
--- a/public/cardapiodata.xlsx
+++ b/public/cardapiodata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\mn-transparency\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0029854E-0062-49F3-BBCC-71A1E8368175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10C97B-7D30-4291-B906-3B2F4121B48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{92F38698-8C92-4FAD-975C-8E92F285CBE1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="205">
   <si>
     <t>Código</t>
   </si>
@@ -63,21 +63,12 @@
     <t>Frango, Peito de Peru</t>
   </si>
   <si>
-    <t>Omeletes e Crepicoas</t>
-  </si>
-  <si>
-    <t>Pão de Queijo</t>
-  </si>
-  <si>
     <t>Coxinha</t>
   </si>
   <si>
     <t>Cachorro Quente</t>
   </si>
   <si>
-    <t>Frango, Requeijão, Carne Seca, Goiabada</t>
-  </si>
-  <si>
     <t>Pao De Queijo</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>1 Pote</t>
   </si>
   <si>
-    <t>Sobremesa Inteira</t>
-  </si>
-  <si>
     <t>Pudim</t>
   </si>
   <si>
@@ -147,21 +135,12 @@
     <t>Torta de Ameixa</t>
   </si>
   <si>
-    <t>Bolo Recheado MN MIx</t>
-  </si>
-  <si>
     <t>Pote da Felicidade</t>
   </si>
   <si>
     <t>Cheesecake</t>
   </si>
   <si>
-    <t>Torta Inteira de Maçã</t>
-  </si>
-  <si>
-    <t>Bolo de Festa</t>
-  </si>
-  <si>
     <t>Sucos Naturais</t>
   </si>
   <si>
@@ -174,24 +153,12 @@
     <t>200 ml</t>
   </si>
   <si>
-    <t>Vitamina de 3 Frutas</t>
-  </si>
-  <si>
-    <t>Vitamina de 2 Frutas</t>
-  </si>
-  <si>
     <t>Frutas a Escolher</t>
   </si>
   <si>
     <t>Chai Latte</t>
   </si>
   <si>
-    <t>Smoothie</t>
-  </si>
-  <si>
-    <t>Soda Italiana</t>
-  </si>
-  <si>
     <t>Cafés &amp; Chocolates</t>
   </si>
   <si>
@@ -228,57 +195,15 @@
     <t>Refeições</t>
   </si>
   <si>
-    <t>Omeletes | Crepiocas Queijo</t>
-  </si>
-  <si>
-    <t>Omeletes | Crepiocas Mista</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (Pre+Mussa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (Pre+Q.Minas)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Minas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mussarela</t>
-  </si>
-  <si>
     <t>Omeletes | Crepiocas</t>
   </si>
   <si>
     <t xml:space="preserve"> Frango +Requeijão</t>
   </si>
   <si>
-    <t xml:space="preserve"> (Fra+Tom Seco+Req)       </t>
-  </si>
-  <si>
-    <t>Nossa Crepioca de Queijo Mussarela combina a cremosidade e o sabor irresistível do queijo com a leveza da massa, oferecendo uma opção deliciosa para qualquer momento.</t>
-  </si>
-  <si>
-    <t>Nossa Crepioca de Queijo Minas traz o autêntico sabor desse queijo tradicional, garantindo uma experiência leve, nutritiva e cheia de qualidade.</t>
-  </si>
-  <si>
-    <t>Nossa Crepioca Mista de Presunto e Mussarela combina o sabor marcante do presunto com a suavidade da mussarela, proporcionando uma refeição equilibrada e deliciosa.</t>
-  </si>
-  <si>
-    <t>Nossa Crepioca Mista de Presunto e Queijo Minas é a escolha perfeita para quem deseja um toque especial de sabor e textura, unindo ingredientes de qualidade.</t>
-  </si>
-  <si>
     <t>Nossa Crepioca de Frango e Requeijão traz o sabor suculento do frango desfiado combinado com a cremosidade do requeijão, criando uma experiência irresistível.</t>
   </si>
   <si>
-    <t>Nossa Crepioca Especial é preparada com uma seleção única de ingredientes, oferecendo um sabor incomparável e uma experiência diferenciada para quem busca algo especial.</t>
-  </si>
-  <si>
-    <t>Omeletes | Crepiocas Simples</t>
-  </si>
-  <si>
-    <t>Omeletes | Crepiocas Especial</t>
-  </si>
-  <si>
     <t>Croissant</t>
   </si>
   <si>
@@ -315,9 +240,6 @@
     <t>Torta de Banoffe</t>
   </si>
   <si>
-    <t>Broa c/Goiabada</t>
-  </si>
-  <si>
     <t>Salada De Frutas</t>
   </si>
   <si>
@@ -333,9 +255,6 @@
     <t>Suco Detox Verde</t>
   </si>
   <si>
-    <t>Suchá</t>
-  </si>
-  <si>
     <t>Suco Energizante</t>
   </si>
   <si>
@@ -495,9 +414,6 @@
     <t>Blend nutritivo de frutas frescas com leite (opcional vegetal), oferecendo proteínas, cálcio e vitaminas essenciais. Uma opção completa para reposição energética e nutricional.</t>
   </si>
   <si>
-    <t>Blend nutritivo de três frutas selecionadas com leite (opcional vegetal), rico em antioxidantes, fibras e nutrientes essenciais. Uma combinação balanceada para máximo benefício nutricional.</t>
-  </si>
-  <si>
     <t>Combinação harmoniosa do nosso café premium com leite parcialmente desnatado, oferecendo uma opção mais leve e cremosa. Rica em antioxidantes e cálcio, uma escolha equilibrada para seu dia.</t>
   </si>
   <si>
@@ -519,18 +435,9 @@
     <t>Fusão harmoniosa de chocolate e café espresso com leite parcialmente desnatado, oferecendo flavonoides do cacau e antioxidantes do café. Uma opção reconfortante com benefícios cognitivos.</t>
   </si>
   <si>
-    <t>Blend refrescante de frutas frescas, iogurte natural e gelo, sem adição de açúcares ou conservantes. Rico em vitaminas, minerais, antioxidantes e probióticos naturais, uma opção nutritiva e refrescante.</t>
-  </si>
-  <si>
-    <t>Bebida refrescante preparada com xarope natural de frutas e água com gás. Uma alternativa mais leve aos refrigerantes convencionais, com sabores autênticos e menos calorias.</t>
-  </si>
-  <si>
     <t>Método de preparo que evidencia as notas aromáticas dos grãos selecionados. O processo de filtragem lenta preserva os óleos essenciais e compostos bioativos, resultando em uma bebida equilibrada e com menor acidez.</t>
   </si>
   <si>
-    <t>Combinação refrescante de chá gelado com sucos naturais de frutas, unindo os antioxidantes do chá com as vitaminas das frutas selecionadas. Sem adição de açúcar, conservantes ou corantes.</t>
-  </si>
-  <si>
     <t>Blend funcional com ingredientes selecionados que auxiliam na digestão, como abacaxi, gengibre e hortelã. Uma opção refrescante que contribui para o conforto digestivo após as refeições.</t>
   </si>
   <si>
@@ -594,9 +501,6 @@
     <t>Massa leve e macia com recheio de doce de leite artesanal, preparado com redução de açúcar em relação à receita tradicional. Uma indulgência ocasional com sabor autêntico.</t>
   </si>
   <si>
-    <t>Criação especial que combina massa macia com recheios selecionados por sua qualidade e sabor distintivo. Uma opção festiva que preserva o equilíbrio entre sabor e valor nutricional.</t>
-  </si>
-  <si>
     <t>Preparado com laranja fresca, aproveitando a casca rica em óleos essenciais e a polpa cheia de vitamina C. Uma opção cítrica e refrescante com menor adição de açúcar refinado.</t>
   </si>
   <si>
@@ -612,12 +516,6 @@
     <t>Combinação clássica de chocolate e coco, fontes de flavonoides e gorduras de cadeia média respectivamente. Preparado com ingredientes selecionados e adoçado com moderação.</t>
   </si>
   <si>
-    <t>Criação exclusiva que combina diversos sabores em camadas harmoniosas, utilizando ingredientes selecionados por sua qualidade e perfil nutricional. Uma opção especial para momentos de celebração.</t>
-  </si>
-  <si>
-    <t>Combinação tradicional da broa de milho, rica em fibras, com goiabada artesanal, fonte de vitamina C e licopeno. Uma fusão de sabores autênticos com ingredientes de qualidade.</t>
-  </si>
-  <si>
     <t>Sobremesa refrescante em camadas, com abacaxi rico em bromelina, enzima digestiva natural, e creme leve preparado com ingredientes selecionados. Uma opção tropical para finalizar sua refeição.</t>
   </si>
   <si>
@@ -642,9 +540,6 @@
     <t>Sobremesa refrescante com polpa de maracujá, rica em vitaminas e compostos relaxantes naturais. A base crocante e o recheio cremoso criam um contraste perfeito de texturas e sabores.</t>
   </si>
   <si>
-    <t>Versão ampliada da nossa torta individual de maçã, mantendo o mesmo padrão de qualidade e perfil nutricional. Ideal para compartilhar em eventos e celebrações especiais.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Seleção equilibrada de queijos em uma massa leve e macia, proporcionando proteínas e cálcio de alta qualidade. Preparado com moderação de sódio e ingredientes cuidadosamente selecionados.</t>
   </si>
   <si>
@@ -742,6 +637,9 @@
   </si>
   <si>
     <t>Suco Natural com 3 Frutas</t>
+  </si>
+  <si>
+    <t>Vitamina</t>
   </si>
 </sst>
 </file>
@@ -1179,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2493752C-554F-479C-841E-F450C946588B}">
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,18 +1126,18 @@
         <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -1248,19 +1146,19 @@
         <v>159</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="F3" s="6">
         <v>15.9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -1269,17 +1167,17 @@
         <v>150</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="F4" s="6">
         <v>15.9</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -1288,18 +1186,18 @@
         <v>149</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="6">
         <v>15.9</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -1308,18 +1206,18 @@
         <v>151</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6">
         <v>15.9</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -1328,20 +1226,20 @@
         <v>162</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="6">
         <v>15.9</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -1350,20 +1248,20 @@
         <v>180</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="6">
         <v>14.9</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>7</v>
@@ -1374,21 +1272,21 @@
         <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="8" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="6">
         <v>4.5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1396,21 +1294,21 @@
         <v>64</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="6">
         <v>7.9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1418,21 +1316,21 @@
         <v>69</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="8" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="6">
         <v>9.9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1440,420 +1338,417 @@
         <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="6">
         <v>9.9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="6">
-        <v>10.9</v>
+        <v>4.5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="6">
-        <v>4.5</v>
+        <v>7.9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="6">
-        <v>7.9</v>
+        <v>13.9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="6">
-        <v>13.9</v>
+        <v>9.9</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>193</v>
+      <c r="D17" t="s">
+        <v>106</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="6">
-        <v>9.9</v>
+        <v>6.9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="6">
-        <v>6.9</v>
+        <v>12.9</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" t="s">
-        <v>134</v>
+      <c r="D19" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="6">
-        <v>12.9</v>
+        <v>9.9</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>12.9</v>
+      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>87</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>195</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="6">
-        <v>14.9</v>
+      <c r="F21" s="4">
+        <v>8.5</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>174</v>
+      <c r="D22" t="s">
+        <v>109</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="6">
-        <v>12.9</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="F22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>196</v>
+      <c r="D23" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="6">
-        <v>5.9</v>
+        <v>3.3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>83</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>135</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="F24" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="9" t="s">
-        <v>57</v>
+      <c r="F25" s="9">
+        <v>10.9</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>220</v>
+        <v>140</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="4" t="s">
-        <v>157</v>
+      <c r="D26" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="6">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="6">
-        <v>7.5</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="F27" s="9">
+        <v>12.9</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>123</v>
+        <v>30</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" t="s">
-        <v>137</v>
+      <c r="D28" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="9">
-        <v>10.9</v>
+      <c r="F28" s="4">
+        <v>8.5</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>171</v>
+        <v>37</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="6">
-        <v>2.5</v>
+        <v>12.9</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>186</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="9">
-        <v>12.9</v>
+      <c r="F30" s="6">
+        <v>13.9</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>124</v>
+        <v>20</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" t="s">
+        <v>113</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="4">
-        <v>8.5</v>
+        <v>7.9</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>7</v>
@@ -1861,330 +1756,333 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="6">
-        <v>12.9</v>
+      <c r="F32" s="4">
+        <v>8.5</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" t="s">
-        <v>139</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="6">
-        <v>13.9</v>
+        <v>12.9</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>20</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D34" t="s">
-        <v>140</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="4">
-        <v>7.9</v>
+      <c r="F34" s="6">
+        <v>12.9</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" t="s">
-        <v>141</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="4">
-        <v>8.5</v>
+      <c r="F35" s="6">
+        <v>9.9</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>234</v>
+        <v>187</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="6">
-        <v>12.9</v>
+        <v>6.99</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="6">
-        <v>12.9</v>
+      <c r="F37" s="4">
+        <v>8.5</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="6">
-        <v>9.9</v>
+      <c r="F38" s="4">
+        <v>8.5</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4" t="s">
-        <v>166</v>
+        <v>188</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="6">
-        <v>6.99</v>
+      <c r="F39" s="9">
+        <v>10.9</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>39</v>
+        <v>133</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" t="s">
-        <v>142</v>
+        <v>83</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="E40" s="2"/>
-      <c r="F40" s="4">
-        <v>8.5</v>
+      <c r="F40" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D41" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>116</v>
+      </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="4">
-        <v>8.5</v>
+      <c r="F41" s="6">
+        <v>7.9</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="9">
-        <v>10.9</v>
+        <v>12.5</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>133</v>
+        <v>43</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>110</v>
+        <v>19</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="E43" s="2"/>
-      <c r="F43" s="9" t="s">
-        <v>58</v>
+      <c r="F43" s="4">
+        <v>8.5</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>84</v>
+        <v>145</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="6">
-        <v>7.9</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>30</v>
+        <v>15.9</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>160</v>
+        <v>49</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="G45" s="2" t="s">
+      <c r="F45" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>144</v>
+        <v>84</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="E46" s="2"/>
-      <c r="F46" s="4">
-        <v>8.5</v>
+      <c r="F46" s="9">
+        <v>7.9</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4" t="s">
         <v>145</v>
       </c>
       <c r="E47" s="2"/>
@@ -2192,7 +2090,7 @@
         <v>15.9</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>7</v>
@@ -2200,23 +2098,21 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C48" s="2"/>
       <c r="D48" s="4" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="6">
         <v>15.9</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>7</v>
@@ -2224,41 +2120,41 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="4" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="9">
         <v>7.9</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>212</v>
+        <v>92</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="4" t="s">
-        <v>176</v>
+      <c r="D50" t="s">
+        <v>119</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="6">
         <v>15.9</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>7</v>
@@ -2266,21 +2162,21 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>152</v>
+        <v>48</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="4" t="s">
-        <v>177</v>
+      <c r="D51" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>66</v>
+      <c r="F51" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>7</v>
@@ -2288,63 +2184,67 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>135</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="4" t="s">
-        <v>162</v>
+        <v>16</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="9">
-        <v>7.9</v>
+      <c r="F52" s="4">
+        <v>9.99</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H52" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" t="s">
-        <v>146</v>
+      <c r="D53" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="E53" s="2"/>
-      <c r="F53" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="F53" s="9">
+        <v>12.9</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>206</v>
+        <v>190</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="E54" s="2"/>
-      <c r="F54" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>28</v>
+      <c r="F54" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>7</v>
@@ -2352,91 +2252,85 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>215</v>
+        <v>56</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>216</v>
+        <v>57</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>207</v>
+        <v>58</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="4">
-        <v>9.99</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="E56" s="2"/>
-      <c r="F56" s="9">
-        <v>12.9</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H56" s="2"/>
+      <c r="F56" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>178</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D57" s="10"/>
       <c r="E57" s="2"/>
       <c r="F57" s="6">
         <v>15.9</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
+        <v>50</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="4">
-        <v>16.899999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>7</v>
@@ -2444,23 +2338,21 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="4">
-        <v>19.899999999999999</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>7</v>
@@ -2468,23 +2360,19 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="4">
-        <v>16.899999999999999</v>
+        <v>6.5</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>7</v>
@@ -2492,23 +2380,19 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="4">
-        <v>17.899999999999999</v>
+        <v>7.99</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>7</v>
@@ -2516,23 +2400,19 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>77</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="4">
-        <v>13.9</v>
+        <v>3.2</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>7</v>
@@ -2540,23 +2420,21 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>8</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="4">
-        <v>16.899999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>7</v>
@@ -2564,127 +2442,133 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>6</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="4">
-        <v>10.9</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>7</v>
+      <c r="F64" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="4" t="s">
-        <v>179</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2" t="s">
-        <v>7</v>
+        <v>11.5</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D66" s="10"/>
+        <v>165</v>
+      </c>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="E67" s="2"/>
-      <c r="F67" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>7</v>
+      <c r="F67" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>22</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" t="s">
+        <v>120</v>
+      </c>
       <c r="E68" s="2"/>
-      <c r="F68" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>7</v>
+      <c r="F68" s="6">
+        <v>7.9</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>23</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>17</v>
+        <v>169</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D69" s="2"/>
+        <v>179</v>
+      </c>
+      <c r="D69" t="s">
+        <v>121</v>
+      </c>
       <c r="E69" s="2"/>
-      <c r="F69" s="4">
-        <v>2.2000000000000002</v>
+      <c r="F69" s="6">
+        <v>15.9</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>7</v>
@@ -2692,59 +2576,67 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>15</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" t="s">
+        <v>122</v>
+      </c>
       <c r="E70" s="2"/>
       <c r="F70" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H70" s="2" t="s">
+        <v>8.5</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H70" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>14</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>218</v>
+        <v>82</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="D71" t="s">
+        <v>123</v>
+      </c>
       <c r="E71" s="2"/>
-      <c r="F71" s="4">
-        <v>7.99</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>7</v>
+      <c r="F71" s="6">
+        <v>6</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H71" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>13</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>219</v>
+        <v>173</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="D72" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="E72" s="2"/>
-      <c r="F72" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>4</v>
+      <c r="F72" s="6">
+        <v>5</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>7</v>
@@ -2752,707 +2644,395 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>52</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>124</v>
+      </c>
       <c r="E73" s="2"/>
       <c r="F73" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H73" s="2" t="s">
+        <v>7.9</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H73" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>100</v>
+        <v>201</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>197</v>
+        <v>42</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
-      <c r="F74" s="6">
-        <v>12.9</v>
-      </c>
+      <c r="F74" s="6"/>
       <c r="G74" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H74" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>198</v>
+        <v>42</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="6">
-        <v>11.5</v>
+        <v>9.9</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H75" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>92</v>
+        <v>203</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>199</v>
+        <v>42</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="6">
-        <v>14</v>
+        <v>9.9</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H76" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" s="2" t="s">
-        <v>200</v>
+      <c r="D77" t="s">
+        <v>125</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="6">
-        <v>12.9</v>
+        <v>8.9</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H77" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="6">
-        <v>7.9</v>
+        <v>4</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H78" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D79" t="s">
-        <v>148</v>
+        <v>78</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>7</v>
+        <v>8.9</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H79" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" t="s">
-        <v>149</v>
+        <v>76</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="E80" s="2"/>
-      <c r="F80" s="4">
-        <v>8.5</v>
+      <c r="F80" s="6">
+        <v>8.9</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="H80" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="2"/>
+        <v>77</v>
+      </c>
       <c r="D81" t="s">
-        <v>150</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>127</v>
+      </c>
       <c r="F81" s="6">
-        <v>6</v>
+        <v>8.9</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H81" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>173</v>
+        <v>79</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E82" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="D82" t="s">
+        <v>150</v>
+      </c>
       <c r="F82" s="6">
-        <v>5</v>
+        <v>9.9</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
+      </c>
+      <c r="H82" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>18</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" t="s">
-        <v>151</v>
-      </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="4">
-        <v>7.9</v>
+        <v>177</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D83" s="8"/>
+      <c r="F83" s="6">
+        <v>19.899999999999999</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H83" t="s">
+        <v>55</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="9">
-        <v>16</v>
+        <v>70</v>
+      </c>
+      <c r="D84" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="6">
+        <v>14.9</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>55</v>
+        <v>27</v>
+      </c>
+      <c r="H84" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C85" s="2"/>
-      <c r="D85" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E85" s="2"/>
+        <v>196</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="F85" s="6">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="H85" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>114</v>
+        <v>175</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E86" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="F86" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="G86" s="5"/>
+        <v>11.5</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F87" s="6">
+        <v>9.9</v>
+      </c>
       <c r="G87" s="5" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="H87" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="D88" t="s">
+        <v>169</v>
+      </c>
       <c r="F88" s="6">
-        <v>9.9</v>
+        <v>12.5</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H88" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>170</v>
+      </c>
       <c r="F89" s="6">
         <v>9.9</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="H89" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" t="s">
-        <v>152</v>
-      </c>
-      <c r="E90" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="F90" s="6">
-        <v>8.9</v>
+        <v>11.5</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H90" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C91" s="2"/>
+        <v>204</v>
+      </c>
       <c r="D91" t="s">
-        <v>153</v>
-      </c>
-      <c r="E91" s="2"/>
+        <v>128</v>
+      </c>
       <c r="F91" s="6">
-        <v>4</v>
+        <v>8.9</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H91" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>118</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E92" s="2"/>
-      <c r="F92" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H92" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
-        <v>116</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E93" s="2"/>
-      <c r="F93" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H93" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
-        <v>117</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D94" t="s">
-        <v>154</v>
-      </c>
-      <c r="F94" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G94" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H94" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
-        <v>79</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D95" t="s">
-        <v>181</v>
-      </c>
-      <c r="F95" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
-        <v>177</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D96" s="8"/>
-      <c r="F96" s="6">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G96" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H96" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
-        <v>80</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D97" t="s">
-        <v>201</v>
-      </c>
-      <c r="F97" s="6">
-        <v>14.9</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H97" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
-        <v>174</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F98" s="6">
-        <v>15</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H98" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
-        <v>175</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="F99" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="G99" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H99" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
-        <v>77</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F100" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H100" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
-        <v>76</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D101" t="s">
-        <v>203</v>
-      </c>
-      <c r="F101" s="6">
-        <v>12.5</v>
-      </c>
-      <c r="G101" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H101" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
-        <v>78</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F102" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G102" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H102" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
-        <v>176</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="F103" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="G103" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H103" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
-        <v>93</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F104" s="6">
-        <v>135</v>
-      </c>
-      <c r="G104" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H104" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
-        <v>112</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D105" t="s">
-        <v>155</v>
-      </c>
-      <c r="F105" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G105" s="5"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
-        <v>113</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D106" t="s">
-        <v>156</v>
-      </c>
-      <c r="F106" s="6">
-        <v>10.5</v>
-      </c>
-      <c r="G106" s="5"/>
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H106">
-    <sortCondition ref="B2:B106"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H91">
+    <sortCondition ref="B2:B91"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adicionando novas imagens .jpg de itens ao cardapio
</commit_message>
<xml_diff>
--- a/public/cardapiodata.xlsx
+++ b/public/cardapiodata.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\mn-transparency\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10C97B-7D30-4291-B906-3B2F4121B48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E901148-3F87-4990-97AC-ACE51486030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{92F38698-8C92-4FAD-975C-8E92F285CBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$83</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="216">
   <si>
     <t>Código</t>
   </si>
@@ -75,12 +78,6 @@
     <t>Cheddar, Frango, Lombo, Requeijão</t>
   </si>
   <si>
-    <t>Empada Integral</t>
-  </si>
-  <si>
-    <t>Camarão</t>
-  </si>
-  <si>
     <t>Esfiha</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>1 Fatia</t>
   </si>
   <si>
-    <t>1 Pote</t>
-  </si>
-  <si>
     <t>Pudim</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>Carne, Frango, Linguiça</t>
   </si>
   <si>
-    <t>Aipim</t>
-  </si>
-  <si>
     <t>Batata Doce</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>Croissant</t>
   </si>
   <si>
-    <t>Pao De Batata</t>
-  </si>
-  <si>
     <t>Bolo Integral de Banana</t>
   </si>
   <si>
@@ -291,15 +279,6 @@
     <t>Lasanha de Abobrinha</t>
   </si>
   <si>
-    <t>Arroz Com Sobrecoxa</t>
-  </si>
-  <si>
-    <t>Arroz Com Frango Desfiado</t>
-  </si>
-  <si>
-    <t>Arroz Com Strogonoff</t>
-  </si>
-  <si>
     <t>Macarrão Proteico</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>Saladinha</t>
   </si>
   <si>
-    <t>Torta De Bacalhau</t>
-  </si>
-  <si>
     <t>Cheeseburger</t>
   </si>
   <si>
@@ -372,9 +348,6 @@
     <t>Preparado com massa integral fermentada naturalmente, oferecendo fibras e nutrientes essenciais. Os recheios são preparados com ingredientes de alta qualidade e baixo teor de sódio.</t>
   </si>
   <si>
-    <t>Massa rica em fibras e nutrientes essenciais, com recheios preparados artesanalmente sem conservantes artificiais. O recheio de camarão é fonte de proteínas de alta qualidade e selênio.</t>
-  </si>
-  <si>
     <t>Preparada com gelatina sem açúcar e frutas naturais, oferece proteínas de fácil digestão e antioxidantes. Uma opção leve e refrescante para finalizar sua refeição.</t>
   </si>
   <si>
@@ -480,9 +453,6 @@
     <t>Preparada com bacalhau dessalgado, fonte de proteínas de alta qualidade e ômega-3, combinado com batatas e temperos frescos. A massa é feita com farinha integral para maior aporte de fibras.</t>
   </si>
   <si>
-    <t>Recheio rico em camarão, fonte de proteínas de alta qualidade e selênio, combinado com legumes frescos e temperos naturais. A massa leve e crocante é preparada com ingredientes selecionados.</t>
-  </si>
-  <si>
     <t>Combinação harmoniosa de frango desfiado, fonte de proteínas magras, com requeijão light que adiciona cremosidade com menos gordura. A massa é preparada com farinha integral para maior valor nutricional.</t>
   </si>
   <si>
@@ -540,18 +510,9 @@
     <t>Sobremesa refrescante com polpa de maracujá, rica em vitaminas e compostos relaxantes naturais. A base crocante e o recheio cremoso criam um contraste perfeito de texturas e sabores.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Seleção equilibrada de queijos em uma massa leve e macia, proporcionando proteínas e cálcio de alta qualidade. Preparado com moderação de sódio e ingredientes cuidadosamente selecionados.</t>
-  </si>
-  <si>
     <t>Combinação clássica de presunto magro selecionado e mussarela com teor reduzido de gordura, servido em pão integral rico em fibras. Um lanche equilibrado e satisfatório para qualquer hora do dia.</t>
   </si>
   <si>
-    <t>Massa macia e saborosa elaborada com batata, fonte de carboidratos complexos e potássio, recheada com opções proteicas selecionadas. Um lanche nutritivo com perfil de absorção gradual.</t>
-  </si>
-  <si>
-    <t>Massa Cheese</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aipim, Batata Doce, Abóbora, Frango </t>
   </si>
   <si>
@@ -615,9 +576,6 @@
     <t>Torta de Palmito</t>
   </si>
   <si>
-    <t>Torta de Camarao</t>
-  </si>
-  <si>
     <t>Doce de Frutas Vermelhas</t>
   </si>
   <si>
@@ -640,6 +598,84 @@
   </si>
   <si>
     <t>Vitamina</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Torta de Bacalhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torta de Quiche </t>
+  </si>
+  <si>
+    <t>Alho Poró</t>
+  </si>
+  <si>
+    <t>Empadão</t>
+  </si>
+  <si>
+    <t>Aveia, Grão de bico</t>
+  </si>
+  <si>
+    <t>Arroz com Carne Assada</t>
+  </si>
+  <si>
+    <t>Arroz com Frango Desfiado</t>
+  </si>
+  <si>
+    <t>Arroz com Sobrecoxa</t>
+  </si>
+  <si>
+    <t>Arroz com Strogonoff</t>
+  </si>
+  <si>
+    <t>Arroz com Tilapia</t>
+  </si>
+  <si>
+    <t>Arroz com Feijoada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolo de Milho </t>
+  </si>
+  <si>
+    <t>Bolo Mesclado</t>
+  </si>
+  <si>
+    <t>Pavê de Limão</t>
+  </si>
+  <si>
+    <t>Delicia de Maracuja</t>
+  </si>
+  <si>
+    <t>Preparado com massa integral rica em fibras e recheios nutritivos selecionados. Nossa versão utiliza aveia ou grão de bico como base, aumentando o aporte proteico e de fibras. Os recheios são preparados com ingredientes frescos e temperos naturais, sem conservantes artificiais.</t>
+  </si>
+  <si>
+    <t>Combinação balanceada de carboidratos complexos do arroz integral com proteínas magras da tilápia, peixe rico em ômega-3 e com baixo teor de gordura. Preparado com temperos naturais e ervas frescas, oferece aminoácidos essenciais e ácidos graxos benéficos para a saúde cardiovascular.</t>
+  </si>
+  <si>
+    <t>Versão mais leve da tradicional feijoada, utilizando cortes magros de carne e feijão preto rico em fibras, ferro e proteínas vegetais. O arroz integral adiciona carboidratos complexos e fibras, resultando em uma refeição nutritiva com menor teor de gordura saturada.</t>
+  </si>
+  <si>
+    <t>Preparado com farinha de milho integral, fonte natural de fibras e carboidratos complexos. Nossa receita utiliza menos açúcar refinado e incorpora o milho fresco, rico em antioxidantes como luteína e zeaxantina, importantes para a saúde ocular.</t>
+  </si>
+  <si>
+    <t>Combinação harmoniosa de ingredientes nutritivos, unindo diferentes farinhas integrais para aumentar o aporte de fibras e nutrientes. Preparado com redução de açúcar e adição de frutas naturais, oferecendo antioxidantes e vitaminas essenciais.</t>
+  </si>
+  <si>
+    <t>Sobremesa refrescante preparada com limão fresco rico em vitamina C e flavonoides cítricos. Nossa versão utiliza creme light e redução de açúcar, mantendo o sabor marcante do limão enquanto oferece benefícios antioxidantes e menor teor calórico.</t>
+  </si>
+  <si>
+    <t>Sobremesa tropical rica em vitamina C e compostos bioativos do maracujá, fruta conhecida por suas propriedades calmantes naturais. Preparada com polpa natural da fruta, oferece fibras e antioxidantes com sabor exótico irresistível.</t>
+  </si>
+  <si>
+    <t>Preparada com bacalhau dessalgado, fonte de proteínas magras e ômega-3. A massa leve e os vegetais frescos adicionam fibras e nutrientes essenciais. Rica em fósforo e vitaminas do complexo B, importantes para o sistema nervoso e saúde óssea.</t>
+  </si>
+  <si>
+    <t>Nossa versão utiliza massa integral e recheio com ovos caipiras, fonte de proteínas completas e colina. Os vegetais frescos adicionam fibras, vitaminas e minerais. Preparada com leite desnatado e queijos com menor teor de gordura, resultando em uma opção mais equilibrada nutricionalmente.</t>
+  </si>
+  <si>
+    <t>Marmitinha - Aipim</t>
   </si>
 </sst>
 </file>
@@ -687,7 +723,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -710,22 +746,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -733,7 +758,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,7 +766,11 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,21 +1105,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2493752C-554F-479C-841E-F450C946588B}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1111,7 +1139,7 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1126,423 +1154,473 @@
         <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="9" t="s">
-        <v>45</v>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>159</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5">
         <v>15.9</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>149</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>88</v>
+      <c r="A5" s="12">
+        <v>187</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="6">
+      <c r="D5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F5" s="5">
         <v>15.9</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="6">
+      <c r="D6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" s="5">
         <v>15.9</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6">
+        <v>198</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="5">
         <v>15.9</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="6">
-        <v>14.9</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>55</v>
+        <v>199</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>73</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>34</v>
+      <c r="A9" s="12">
+        <v>186</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6">
-        <v>4.5</v>
+      <c r="D9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="4">
+        <v>17.989999999999998</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="6">
-        <v>7.9</v>
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="5">
+        <v>15.9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>69</v>
+        <v>180</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6">
-        <v>9.9</v>
+        <v>89</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="5">
+        <v>14.9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="6">
-        <v>9.9</v>
+      <c r="D12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4.5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="6">
-        <v>4.5</v>
+        <v>144</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="5">
+        <v>7.9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="6">
-        <v>7.9</v>
+      <c r="D14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F14" s="5">
+        <v>9.9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="6">
-        <v>13.9</v>
+        <v>146</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F15" s="5">
+        <v>9.9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="6">
-        <v>9.9</v>
+        <v>147</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16" s="5">
+        <v>4.5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="6">
-        <v>6.9</v>
+      <c r="D17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="5">
+        <v>7.9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>70</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>65</v>
+      <c r="A18" s="12">
+        <v>188</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>202</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="6">
-        <v>12.9</v>
-      </c>
+      <c r="D18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="6">
-        <v>9.9</v>
+        <v>149</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="5">
+        <v>13.9</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>182</v>
+        <v>71</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="6">
-        <v>12.9</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>63</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4">
-        <v>8.5</v>
+        <v>97</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="5">
+        <v>6.9</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>25</v>
@@ -1553,139 +1631,167 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="9" t="s">
-        <v>46</v>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F22" s="5">
+        <v>12.9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>143</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>185</v>
+      <c r="A23" s="12">
+        <v>189</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="6">
-        <v>3.3</v>
+      <c r="D23" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="6">
-        <v>7.5</v>
-      </c>
-      <c r="G24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H24" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="9">
-        <v>10.9</v>
+      <c r="D25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F25" s="5">
+        <v>12.9</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>115</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>140</v>
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="6">
-        <v>2.5</v>
+        <v>99</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F26" s="4">
+        <v>8.5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="9">
-        <v>12.9</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4">
-        <v>8.5</v>
+      <c r="D28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F28" s="5">
+        <v>3.3</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>7</v>
@@ -1693,62 +1799,67 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="6">
-        <v>12.9</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F29" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>186</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="6">
-        <v>13.9</v>
+      <c r="D30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F30" s="8">
+        <v>10.9</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>20</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="4">
-        <v>7.9</v>
+        <v>115</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2.5</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>7</v>
@@ -1756,23 +1867,23 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="4">
-        <v>8.5</v>
+        <v>40</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F32" s="8">
+        <v>12.9</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>7</v>
@@ -1780,122 +1891,140 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>199</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="6">
-        <v>12.9</v>
+      <c r="D33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F33" s="4">
+        <v>8.5</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>197</v>
+        <v>34</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="6">
+      <c r="E34" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" s="5">
         <v>12.9</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="6">
-        <v>9.9</v>
+      <c r="D35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F35" s="5">
+        <v>13.9</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>137</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="6">
-        <v>6.99</v>
+        <v>20</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F36" s="4">
+        <v>7.9</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H36" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="F37" s="4">
         <v>8.5</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>176</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="4">
-        <v>8.5</v>
+      <c r="E38" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F38" s="5">
+        <v>12.9</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>25</v>
@@ -1904,103 +2033,115 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>126</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>188</v>
-      </c>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>191</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="9">
-        <v>10.9</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F39" s="4"/>
       <c r="G39" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H39" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="9" t="s">
-        <v>47</v>
+        <v>182</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" s="5">
+        <v>12.9</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" t="s">
-        <v>116</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="6">
-        <v>7.9</v>
+      <c r="F41" s="5">
+        <v>9.9</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="9">
-        <v>12.5</v>
+        <v>173</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F42" s="5">
+        <v>6.99</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>43</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>19</v>
+      <c r="A43" s="12">
+        <v>184</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E43" s="2"/>
+        <v>206</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="F43" s="4">
-        <v>8.5</v>
+        <v>15.9</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>7</v>
@@ -2008,23 +2149,23 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>55</v>
+        <v>162</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>7</v>
@@ -2032,23 +2173,23 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>55</v>
+        <v>174</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F45" s="8">
+        <v>10.9</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>7</v>
@@ -2056,41 +2197,47 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="9">
-        <v>7.9</v>
+      <c r="D46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H46" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>55</v>
+      <c r="D47" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F47" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>7</v>
@@ -2098,21 +2245,23 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>55</v>
+      <c r="D48" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" s="8">
+        <v>12.5</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>7</v>
@@ -2120,41 +2269,51 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="9">
-        <v>7.9</v>
+        <v>17</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8.5</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H49" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="6">
+        <v>82</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="5">
         <v>15.9</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>55</v>
+      <c r="G50" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>7</v>
@@ -2162,21 +2321,25 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="4">
-        <v>8.5</v>
+        <v>46</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51" s="5">
+        <v>15.9</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>7</v>
@@ -2184,23 +2347,23 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>16</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="4">
-        <v>9.99</v>
+        <v>134</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F52" s="8">
+        <v>7.9</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>7</v>
@@ -2208,43 +2371,47 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="9">
-        <v>12.9</v>
+      <c r="E53" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="5">
+        <v>15.9</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H53" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="6">
+        <v>136</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F54" s="5">
         <v>15.9</v>
       </c>
-      <c r="G54" s="5" t="s">
-        <v>55</v>
+      <c r="G54" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>7</v>
@@ -2252,85 +2419,97 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>11</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="4">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="G55" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F55" s="8">
+        <v>7.9</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="H55" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>192</v>
+        <v>84</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="6">
+      <c r="D56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F56" s="5">
         <v>15.9</v>
       </c>
-      <c r="G56" s="2"/>
+      <c r="G56" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H56" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>156</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>93</v>
+        <v>16</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="6">
-        <v>15.9</v>
-      </c>
-      <c r="G57" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="4">
+        <v>9.99</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="H57" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="4">
-        <v>8.5</v>
+        <v>81</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F58" s="8">
+        <v>12.9</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>7</v>
@@ -2338,21 +2517,25 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>22</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>14</v>
+        <v>167</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="4">
-        <v>2.2000000000000002</v>
+        <v>177</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F59" s="5">
+        <v>15.9</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>7</v>
@@ -2360,81 +2543,89 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="F60" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G60" s="2"/>
       <c r="H60" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>14</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>183</v>
+        <v>155</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="4">
-        <v>7.99</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="D61" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>13</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="11"/>
+      <c r="E62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F62" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G62" s="2"/>
       <c r="H62" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>52</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="4">
-        <v>8.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>7</v>
@@ -2442,130 +2633,126 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>88</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>163</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="6">
-        <v>12.9</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H64" t="s">
-        <v>29</v>
+      <c r="F64" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>74</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>164</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H65" t="s">
-        <v>28</v>
+      <c r="F65" s="4">
+        <v>7.99</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>75</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="6">
-        <v>14</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H66" t="s">
-        <v>28</v>
+      <c r="F66" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
-        <v>166</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="E67" s="2"/>
-      <c r="F67" s="6">
-        <v>12.9</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H67" t="s">
-        <v>29</v>
+      <c r="F67" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="6">
-        <v>7.9</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H68" t="s">
-        <v>28</v>
+      <c r="D68" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F68" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>169</v>
+        <v>74</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D69" t="s">
-        <v>121</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="6">
-        <v>15.9</v>
+        <v>185</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F69" s="5">
+        <v>11.5</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>25</v>
@@ -2575,68 +2762,72 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>62</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D70" t="s">
-        <v>122</v>
-      </c>
-      <c r="E70" s="2"/>
+      <c r="A70" s="12">
+        <v>190</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="F70" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="G70" s="5" t="s">
+        <v>12.9</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" t="s">
-        <v>123</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="6">
-        <v>6</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" t="s">
-        <v>29</v>
+      <c r="D71" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F71" s="5">
+        <v>14</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>173</v>
+        <v>89</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="6">
-        <v>5</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>55</v>
+      <c r="D72" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F72" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>7</v>
@@ -2644,395 +2835,587 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>18</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" t="s">
-        <v>124</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="4">
+        <v>85</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F73" s="5">
         <v>7.9</v>
       </c>
-      <c r="G73" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H73" t="s">
+      <c r="G73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="5" t="s">
-        <v>38</v>
+        <v>165</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F74" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H75" t="s">
-        <v>40</v>
+        <v>91</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F75" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H76" t="s">
-        <v>40</v>
+        <v>66</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F76" s="5">
+        <v>6</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>119</v>
+        <v>173</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" t="s">
-        <v>125</v>
-      </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H77" t="s">
-        <v>39</v>
+      <c r="D77" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F77" s="5">
+        <v>5</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>109</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" t="s">
-        <v>126</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="6">
+        <v>18</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F78" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G78" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H78" t="s">
-        <v>41</v>
+      <c r="H78" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="6">
+        <v>115</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F79" s="5">
         <v>8.9</v>
       </c>
-      <c r="G79" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H79" t="s">
-        <v>39</v>
+      <c r="G79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="6">
-        <v>8.9</v>
-      </c>
-      <c r="G80" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F80" s="5">
+        <v>4</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H80" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F81" s="6">
+      <c r="E81" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F81" s="5">
         <v>8.9</v>
       </c>
-      <c r="G81" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H81" t="s">
-        <v>39</v>
+      <c r="G81" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F82" s="5">
+        <v>8.9</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D82" t="s">
-        <v>150</v>
-      </c>
-      <c r="F82" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H82" t="s">
-        <v>28</v>
+      <c r="H82" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="F83" s="6">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>55</v>
+        <v>186</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="9"/>
+      <c r="E83" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="5">
+        <v>4.8</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D84" t="s">
-        <v>167</v>
-      </c>
-      <c r="F84" s="6">
-        <v>14.9</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H84" t="s">
-        <v>28</v>
+        <v>187</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>174</v>
+        <v>107</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F85" s="6">
-        <v>15</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>55</v>
+        <v>188</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>175</v>
+        <v>117</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F86" s="6">
-        <v>11.5</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F86" s="5">
+        <v>8.9</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F87" s="6">
+        <v>32</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F87" s="5">
         <v>9.9</v>
       </c>
-      <c r="G87" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H87" t="s">
-        <v>28</v>
+      <c r="G87" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D88" t="s">
-        <v>169</v>
-      </c>
-      <c r="F88" s="6">
-        <v>12.5</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H88" t="s">
-        <v>28</v>
+        <v>191</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F88" s="5">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F89" s="6">
-        <v>9.9</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H89" t="s">
-        <v>28</v>
+        <v>65</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F89" s="5">
+        <v>14.9</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F90" s="6">
+        <v>179</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F90" s="5">
         <v>11.5</v>
       </c>
-      <c r="G90" s="5" t="s">
-        <v>55</v>
+      <c r="G90" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
+        <v>77</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F91" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>76</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F92" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>78</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F93" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>176</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F94" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>183</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F95" s="5">
+        <v>140</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
         <v>112</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D91" t="s">
-        <v>128</v>
-      </c>
-      <c r="F91" s="6">
+      <c r="B96" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F96" s="5">
         <v>8.9</v>
       </c>
-      <c r="G91" s="5" t="s">
-        <v>27</v>
+      <c r="G96" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H91">
-    <sortCondition ref="B2:B91"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H89">
+    <sortCondition ref="B2:B89"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create a new nav for filter and news images
</commit_message>
<xml_diff>
--- a/public/cardapiodata.xlsx
+++ b/public/cardapiodata.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\mn-transparency\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinopc\Project\mn-transparency\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E901148-3F87-4990-97AC-ACE51486030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFB3F35-8688-4916-8908-885E4834847E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{92F38698-8C92-4FAD-975C-8E92F285CBE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{92F38698-8C92-4FAD-975C-8E92F285CBE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$97</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="233">
   <si>
     <t>Código</t>
   </si>
@@ -186,12 +186,6 @@
     <t>Refeições</t>
   </si>
   <si>
-    <t>Omeletes | Crepiocas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Frango +Requeijão</t>
-  </si>
-  <si>
     <t>Nossa Crepioca de Frango e Requeijão traz o sabor suculento do frango desfiado combinado com a cremosidade do requeijão, criando uma experiência irresistível.</t>
   </si>
   <si>
@@ -522,12 +516,6 @@
     <t>Macarrao Bolonhesa com salada</t>
   </si>
   <si>
-    <t xml:space="preserve">Quibe </t>
-  </si>
-  <si>
-    <t>, Queijo e Presunto, Ricota</t>
-  </si>
-  <si>
     <t>Misto Quente</t>
   </si>
   <si>
@@ -561,9 +549,6 @@
     <t>Nhoque</t>
   </si>
   <si>
-    <t>Frbngo, Carne</t>
-  </si>
-  <si>
     <t>Panqueca de Aveia</t>
   </si>
   <si>
@@ -600,9 +585,6 @@
     <t>Vitamina</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Torta de Bacalhau</t>
   </si>
   <si>
@@ -676,13 +658,82 @@
   </si>
   <si>
     <t>Marmitinha - Aipim</t>
+  </si>
+  <si>
+    <t>Quibe</t>
+  </si>
+  <si>
+    <t>Queijo e Presunto, Ricota</t>
+  </si>
+  <si>
+    <t>Combinação equilibrada de carboidratos complexos do arroz integral com proteínas de alta qualidade da carne assada. O método de preparo assado preserva nutrientes e reduz a adição de gorduras, oferecendo ferro heme de fácil absorção e aminoácidos essenciais para manutenção muscular.</t>
+  </si>
+  <si>
+    <t>Sobremesa tradicional preparada com milho branco, fonte de fibras e carboidratos complexos. O coco adiciona gorduras saudáveis (triglicerídeos de cadeia média) e sabor tropical. Nossa versão utiliza leite desnatado e açúcar mascavo, resultando em uma opção mais nutritiva e com menor índice glicêmico.</t>
+  </si>
+  <si>
+    <t>Sobremesa cremosa preparada com cream cheese light e base de biscoito integral. Rica em proteínas lácteas e cálcio, nossa versão utiliza adoçantes naturais e frutas frescas como cobertura, oferecendo antioxidantes e reduzindo o teor calórico total.</t>
+  </si>
+  <si>
+    <t>Sobremesa natural rica em potássio, vitamina B6 e fibras prebióticas da banana. Preparada com frutas maduras que dispensam açúcar adicionado, oferece energia natural e nutrientes que auxiliam na função muscular e regulação da pressão arterial.</t>
+  </si>
+  <si>
+    <t>Combinação de frutas vermelhas ricas em antocianinas, poderosos antioxidantes com propriedades anti-inflamatórias. Preparado com frutas frescas e menor adição de açúcar, oferece vitamina C, fibras e compostos bioativos benéficos para a saúde cardiovascular.</t>
+  </si>
+  <si>
+    <t>Versão mais saudável do clássico sabor, combinando coco e cacau. O coco oferece gorduras saudáveis e fibras, enquanto o cacau fornece flavonoides antioxidantes. Preparado com chocolate meio amargo e açúcar de coco para reduzir o impacto glicêmico.</t>
+  </si>
+  <si>
+    <t>Massa integral fermentada naturalmente, rica em fibras e carboidratos complexos. Os recheios são preparados com carnes magras, temperos naturais e baixo teor de sódio. Uma opção equilibrada que combina proteínas, carboidratos e vegetais em uma refeição prática.</t>
+  </si>
+  <si>
+    <t>Desenvolvida especialmente para dietas com restrição de carboidratos, utiliza farinha de amêndoas e ovos como base. Rica em proteínas de alto valor biológico e gorduras saudáveis, oferece saciedade prolongada sem causar picos de glicemia.</t>
+  </si>
+  <si>
+    <t>Preparado com polvilho azedo e queijo minas, naturalmente sem glúten. Fonte de cálcio e proteínas lácteas, nossos pães de queijo são assados para obter textura crocante por fora e macia por dentro, com recheios nutritivos opcionais.</t>
+  </si>
+  <si>
+    <t>Combinação rica em proteínas completas dos ovos caipiras com fibras do pão integral. Os ovos fornecem todos os aminoácidos essenciais, colina para função cerebral e vitaminas lipossolúveis. Uma opção nutritiva e satisfatória para qualquer refeição.</t>
+  </si>
+  <si>
+    <t>União de fibras do pão integral com proteínas e cálcio do queijo. Preparado quente ou frio, oferece carboidratos complexos de absorção lenta e nutrientes lácteos essenciais. O pão integral adiciona vitaminas do complexo B e minerais.</t>
+  </si>
+  <si>
+    <t>Versão integral do clássico pão na chapa, tostado para realçar sabor e textura. A manteiga com sal adiciona gorduras essenciais e sabor, enquanto o pão integral fornece fibras e energia sustentada. Uma opção reconfortante e nutritiva.</t>
+  </si>
+  <si>
+    <t>Versão assada do tradicional pastel, reduzindo significativamente o teor de gordura. A massa crocante é recheada com ingredientes frescos e proteínas magras. O método de preparo no forno preserva nutrientes e oferece textura satisfatória com menos calorias.</t>
+  </si>
+  <si>
+    <t>Preparado exclusivamente com frutas frescas da estação, sem adição de açúcar, conservantes ou corantes. Preserva vitaminas, minerais e antioxidantes naturais das frutas, oferecendo hidratação saudável e nutrientes biodisponíveis.</t>
+  </si>
+  <si>
+    <t>Combinação sinérgica de duas frutas selecionadas, maximizando o aporte de diferentes vitaminas e antioxidantes. A mistura oferece perfil nutricional mais completo, com sabores complementares e benefícios potencializados para a saúde.</t>
+  </si>
+  <si>
+    <t>Blend premium de três frutas cuidadosamente selecionadas, oferecendo complexo vitamínico amplo e diversidade de antioxidantes. Esta combinação maximiza os benefícios nutricionais, proporcionando hidratação saudável e energia natural sustentada.</t>
+  </si>
+  <si>
+    <t>Omelete</t>
+  </si>
+  <si>
+    <t>Crepioca</t>
+  </si>
+  <si>
+    <t>Frango + Requeijão</t>
+  </si>
+  <si>
+    <t>Contém lactose</t>
+  </si>
+  <si>
+    <t>Não contém lactose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -707,12 +758,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFABB2BF"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -750,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,7 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1105,25 +1149,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2493752C-554F-479C-841E-F450C946588B}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.25" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1149,19 +1193,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>42</v>
@@ -1173,21 +1217,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F3" s="5">
         <v>15.9</v>
@@ -1199,16 +1241,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>185</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>196</v>
+    <row r="4" spans="1:8">
+      <c r="A4" s="11">
+        <v>187</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F4" s="5">
         <v>15.9</v>
       </c>
@@ -1219,19 +1265,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>187</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>201</v>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>150</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>208</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F5" s="5">
         <v>15.9</v>
@@ -1243,19 +1289,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>94</v>
+      <c r="D6" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F6" s="5">
         <v>15.9</v>
@@ -1267,20 +1313,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="5">
         <v>15.9</v>
       </c>
@@ -1291,22 +1335,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>151</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>199</v>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11">
+        <v>186</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="4" t="s">
-        <v>132</v>
+      <c r="D8" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F8" s="5">
-        <v>15.9</v>
+        <v>232</v>
+      </c>
+      <c r="F8" s="4">
+        <v>17.989999999999998</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>51</v>
@@ -1315,22 +1359,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>186</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C9" s="2"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2">
+        <v>162</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>207</v>
+        <v>93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F9" s="4">
-        <v>17.989999999999998</v>
+        <v>232</v>
+      </c>
+      <c r="F9" s="5">
+        <v>15.9</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>51</v>
@@ -1339,24 +1385,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F10" s="5">
-        <v>15.9</v>
+        <v>14.9</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>51</v>
@@ -1365,48 +1411,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
-        <v>180</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F11" s="5">
-        <v>14.9</v>
+        <v>4.5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="4" t="s">
-        <v>143</v>
+      <c r="D12" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F12" s="5">
-        <v>4.5</v>
+        <v>7.9</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>25</v>
@@ -1415,22 +1459,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>144</v>
+      <c r="D13" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F13" s="5">
-        <v>7.9</v>
+        <v>9.9</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
@@ -1439,19 +1483,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="4" t="s">
-        <v>145</v>
+      <c r="D14" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F14" s="5">
         <v>9.9</v>
@@ -1463,22 +1507,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F15" s="5">
-        <v>9.9</v>
+        <v>4.5</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
@@ -1487,22 +1531,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F16" s="5">
-        <v>4.5</v>
+        <v>7.9</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>25</v>
@@ -1511,23 +1555,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>65</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>58</v>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11">
+        <v>188</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>196</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F17" s="5">
-        <v>7.9</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1535,21 +1577,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>188</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>202</v>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>72</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>209</v>
+        <v>147</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>231</v>
+      </c>
+      <c r="F18" s="5">
+        <v>13.9</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1557,22 +1601,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F19" s="5">
-        <v>13.9</v>
+        <v>9.9</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>25</v>
@@ -1581,22 +1625,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F20" s="5">
-        <v>9.9</v>
+        <v>6.9</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>25</v>
@@ -1605,22 +1649,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F21" s="5">
-        <v>6.9</v>
+        <v>12.9</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>25</v>
@@ -1629,22 +1673,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>70</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>60</v>
+    <row r="22" spans="1:8">
+      <c r="A22" s="11">
+        <v>189</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F22" s="5">
-        <v>12.9</v>
+        <v>231</v>
+      </c>
+      <c r="F22" s="4">
+        <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>25</v>
@@ -1653,22 +1697,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>189</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>203</v>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2">
+        <v>68</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>210</v>
+        <v>149</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5</v>
+        <v>231</v>
+      </c>
+      <c r="F23" s="5">
+        <v>9.9</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>25</v>
@@ -1677,94 +1721,94 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F24" s="5">
-        <v>9.9</v>
+        <v>12.9</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
-        <v>182</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F25" s="5">
-        <v>12.9</v>
+        <v>231</v>
+      </c>
+      <c r="F25" s="4">
+        <v>8.5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
-        <v>21</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>13</v>
+        <v>121</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="4">
-        <v>8.5</v>
+        <v>231</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>76</v>
+        <v>167</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>100</v>
+      <c r="D27" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>43</v>
+        <v>231</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3.3</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>41</v>
@@ -1773,66 +1817,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="4" t="s">
-        <v>119</v>
+      <c r="D28" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F28" s="5">
-        <v>3.3</v>
+        <v>7.5</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2">
+        <v>123</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="8">
+        <v>10.9</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>83</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F29" s="5">
-        <v>7.5</v>
-      </c>
-      <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F30" s="8">
-        <v>10.9</v>
+        <v>231</v>
+      </c>
+      <c r="F30" s="5">
+        <v>2.5</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>41</v>
@@ -1841,22 +1889,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F31" s="5">
-        <v>2.5</v>
+        <v>231</v>
+      </c>
+      <c r="F31" s="8">
+        <v>12.9</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>41</v>
@@ -1865,141 +1913,145 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F32" s="8">
-        <v>12.9</v>
+        <v>231</v>
+      </c>
+      <c r="F32" s="4">
+        <v>8.5</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>88</v>
+        <v>214</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F33" s="4">
-        <v>8.5</v>
+        <v>231</v>
+      </c>
+      <c r="F33" s="5">
+        <v>12.9</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2">
+        <v>138</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="2">
+        <v>20</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>90</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F34" s="5">
-        <v>12.9</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>138</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F35" s="5">
-        <v>13.9</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
-        <v>20</v>
+        <v>182</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>12</v>
+        <v>229</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>161</v>
+        <v>230</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F36" s="4">
-        <v>7.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
         <v>31</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F37" s="4">
         <v>8.5</v>
@@ -2011,17 +2063,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="16.5" customHeight="1">
       <c r="A38" s="2">
         <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="E38" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F38" s="5">
         <v>12.9</v>
@@ -2033,19 +2087,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+    <row r="39" spans="1:8">
+      <c r="A39" s="11">
         <v>191</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>205</v>
+      <c r="B39" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="2" t="s">
@@ -2055,17 +2109,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="2">
         <v>92</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="E40" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F40" s="5">
         <v>12.9</v>
@@ -2077,16 +2133,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="2">
         <v>91</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="F41" s="5">
         <v>9.9</v>
       </c>
@@ -2097,19 +2157,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
         <v>137</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F42" s="5">
         <v>6.99</v>
@@ -2121,21 +2181,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
+    <row r="43" spans="1:8">
+      <c r="A43" s="11">
         <v>184</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>194</v>
+      <c r="B43" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F43" s="4">
         <v>15.9</v>
@@ -2147,7 +2207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -2155,11 +2215,13 @@
         <v>16</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D44" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="E44" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F44" s="4">
         <v>8.5</v>
@@ -2171,19 +2233,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="2">
         <v>126</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F45" s="8">
         <v>10.9</v>
@@ -2195,19 +2257,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>133</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>44</v>
@@ -2219,19 +2281,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="2">
         <v>84</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F47" s="5">
         <v>7.9</v>
@@ -2243,19 +2305,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="2">
         <v>131</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F48" s="8">
         <v>12.5</v>
@@ -2267,7 +2329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="2">
         <v>43</v>
       </c>
@@ -2278,10 +2340,10 @@
         <v>19</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F49" s="4">
         <v>8.5</v>
@@ -2293,21 +2355,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="2">
         <v>145</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F50" s="5">
         <v>15.9</v>
@@ -2319,7 +2381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="2">
         <v>147</v>
       </c>
@@ -2330,10 +2392,10 @@
         <v>45</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F51" s="5">
         <v>15.9</v>
@@ -2345,19 +2407,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="2">
         <v>134</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F52" s="8">
         <v>7.9</v>
@@ -2369,19 +2431,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="2">
         <v>153</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F53" s="5">
         <v>15.9</v>
@@ -2393,19 +2455,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="2">
         <v>152</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F54" s="5">
         <v>15.9</v>
@@ -2417,19 +2479,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="2">
         <v>135</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F55" s="8">
         <v>7.9</v>
@@ -2441,19 +2503,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="2"/>
+        <v>209</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D56" s="2" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F56" s="5">
         <v>15.9</v>
@@ -2465,164 +2529,174 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" s="2">
+        <v>154</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F57" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="2">
         <v>16</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="B58" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F58" s="4">
+        <v>9.99</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="2">
+        <v>136</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59" s="8">
+        <v>12.9</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="2">
         <v>167</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F57" s="4">
-        <v>9.99</v>
-      </c>
-      <c r="G57" s="2" t="s">
+      <c r="B60" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F60" s="5">
+        <v>15.9</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="2">
+        <v>11</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F61" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="H61" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="2">
+        <v>155</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F58" s="8">
-        <v>12.9</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>167</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F59" s="5">
-        <v>15.9</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>11</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F60" s="4">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>155</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F61" s="5">
-        <v>15.9</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>156</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="11"/>
       <c r="E62" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F62" s="5">
         <v>15.9</v>
       </c>
-      <c r="G62" s="2"/>
+      <c r="G62" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="H62" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="2">
-        <v>22</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>14</v>
+        <v>156</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="4">
-        <v>2.2000000000000002</v>
+        <v>47</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F63" s="5">
+        <v>15.9</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>4</v>
@@ -2631,18 +2705,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="2">
+        <v>22</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="F64" s="4">
-        <v>6.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>4</v>
@@ -2651,18 +2731,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="F65" s="4">
-        <v>7.99</v>
+        <v>6.5</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>4</v>
@@ -2671,18 +2755,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="F66" s="4">
-        <v>3.2</v>
+        <v>7.99</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>4</v>
@@ -2691,68 +2779,72 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="2">
+        <v>13</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F67" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="2">
         <v>52</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="4">
+      <c r="D68" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F68" s="4">
         <v>8.5</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="H68" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="2">
         <v>88</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F68" s="5">
-        <v>12.9</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>74</v>
-      </c>
       <c r="B69" s="4" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F69" s="5">
-        <v>11.5</v>
+        <v>12.9</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>25</v>
@@ -2761,22 +2853,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="12">
-        <v>190</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>204</v>
+    <row r="70" spans="1:8">
+      <c r="A70" s="2">
+        <v>74</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>211</v>
+        <v>151</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F70" s="4">
-        <v>12.9</v>
+        <v>231</v>
+      </c>
+      <c r="F70" s="5">
+        <v>11.5</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>25</v>
@@ -2785,22 +2877,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>75</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>62</v>
+    <row r="71" spans="1:8">
+      <c r="A71" s="11">
+        <v>190</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>198</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F71" s="5">
-        <v>14</v>
+        <v>231</v>
+      </c>
+      <c r="F71" s="4">
+        <v>12.9</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>25</v>
@@ -2809,22 +2901,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72" s="2">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F72" s="5">
-        <v>12.9</v>
+        <v>14</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>25</v>
@@ -2833,22 +2925,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73" s="2">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F73" s="5">
-        <v>7.9</v>
+        <v>12.9</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>25</v>
@@ -2857,50 +2949,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74" s="2">
+        <v>85</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F74" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="2">
         <v>169</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F74" s="5">
+      <c r="B75" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F75" s="5">
         <v>15.9</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
-        <v>62</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F75" s="4">
-        <v>8.5</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>23</v>
@@ -2909,165 +2999,167 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76" s="2">
+        <v>62</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F76" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="2">
         <v>82</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F76" s="5">
+      <c r="B77" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F77" s="5">
         <v>6</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="H77" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="2">
         <v>173</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F77" s="5">
+      <c r="B78" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F78" s="5">
         <v>5</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H77" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="H78" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="2">
         <v>18</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F78" s="4">
+      <c r="D79" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F79" s="4">
         <v>7.9</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="H79" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="2">
         <v>119</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F79" s="5">
-        <v>8.9</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H79" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>109</v>
-      </c>
       <c r="B80" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F80" s="5">
-        <v>4</v>
+        <v>8.9</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="2">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F81" s="5">
-        <v>8.9</v>
+        <v>4</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="2">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C82" s="2"/>
-      <c r="D82" s="2" t="s">
-        <v>128</v>
+      <c r="D82" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F82" s="5">
         <v>8.9</v>
@@ -3079,44 +3171,48 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83" s="2">
-        <v>176</v>
+        <v>116</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D83" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="E83" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F83" s="5">
-        <v>4.8</v>
+        <v>8.9</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="2">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="D84" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F84" s="5">
-        <v>9.9</v>
+        <v>4.8</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>35</v>
@@ -3125,18 +3221,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8">
       <c r="A85" s="2">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="D85" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F85" s="5">
         <v>9.9</v>
       </c>
@@ -3147,166 +3247,168 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8">
       <c r="A86" s="2">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2" t="s">
-        <v>117</v>
+        <v>183</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>227</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F86" s="5">
-        <v>8.9</v>
+        <v>9.9</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H86" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="2">
+        <v>117</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F87" s="5">
+        <v>8.9</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+    <row r="88" spans="1:8">
+      <c r="A88" s="2">
         <v>79</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F87" s="5">
+      <c r="C88" s="2"/>
+      <c r="D88" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F88" s="5">
         <v>9.9</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>174</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F88" s="5">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8">
       <c r="A89" s="2">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="9" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F89" s="5">
-        <v>14.9</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8">
       <c r="A90" s="2">
-        <v>175</v>
+        <v>80</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>179</v>
+        <v>63</v>
       </c>
       <c r="C90" s="2"/>
-      <c r="D90" s="10" t="s">
-        <v>141</v>
+      <c r="D90" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F90" s="5">
-        <v>11.5</v>
+        <v>14.9</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8">
       <c r="A91" s="2">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="10" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F91" s="5">
-        <v>9.9</v>
+        <v>11.5</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8">
       <c r="A92" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>180</v>
+        <v>61</v>
       </c>
       <c r="C92" s="2"/>
-      <c r="D92" s="9" t="s">
-        <v>158</v>
+      <c r="D92" s="10" t="s">
+        <v>155</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F92" s="5">
-        <v>12.5</v>
+        <v>9.9</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>25</v>
@@ -3315,22 +3417,22 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="2">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="C93" s="2"/>
-      <c r="D93" s="10" t="s">
-        <v>159</v>
+      <c r="D93" s="9" t="s">
+        <v>156</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F93" s="5">
-        <v>9.9</v>
+        <v>12.5</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>25</v>
@@ -3339,83 +3441,112 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8">
       <c r="A94" s="2">
-        <v>176</v>
+        <v>78</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>181</v>
+        <v>62</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="10" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F94" s="5">
-        <v>11.5</v>
+        <v>9.9</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8">
       <c r="A95" s="2">
+        <v>176</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F95" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="2">
         <v>183</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F95" s="5">
+      <c r="B96" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F96" s="5">
         <v>140</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H95" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="H96" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="2">
         <v>112</v>
       </c>
-      <c r="B96" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C96" s="2"/>
-      <c r="D96" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F96" s="5">
+      <c r="B97" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F97" s="5">
         <v>8.9</v>
       </c>
-      <c r="G96" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H96" s="2" t="s">
+      <c r="H97" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H89">
-    <sortCondition ref="B2:B89"/>
+  <autoFilter ref="A1:H97" xr:uid="{2493752C-554F-479C-841E-F450C946588B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H97">
+      <sortCondition ref="B1:B97"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H90">
+    <sortCondition ref="B2:B90"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change names on github and Excel
</commit_message>
<xml_diff>
--- a/public/cardapiodata.xlsx
+++ b/public/cardapiodata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dinopc\Project\mn-transparency\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15933E93-17BE-4681-8067-045CF3BBAFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E106C37C-A8CA-4E1E-8FDB-44D583344BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{577F66C6-292F-4C95-80EB-D853036281F5}"/>
   </bookViews>
@@ -177,9 +177,6 @@
     <t>Combinação fresca de frutas sazonais, rica em vitaminas, minerais, fibras e antioxidantes naturais. Sem adição de açúcar, preservando o sabor natural e os benefícios nutricionais das frutas.</t>
   </si>
   <si>
-    <t>Salada De Frutas</t>
-  </si>
-  <si>
     <t>Salgados Integrais</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Composição em camadas de ingredientes selecionados que proporcionam uma experiência sensorial completa. Combinação equilibrada de texturas e sabores para um momento de prazer consciente.</t>
   </si>
   <si>
-    <t>Pote da Felicidade</t>
-  </si>
-  <si>
     <t>Versão sofisticada com nozes selecionadas, ricas em ômega-3 e antioxidantes, combinadas com creme suave e camadas crocantes. Uma indulgência nutritiva preparada com ingredientes premium.</t>
   </si>
   <si>
@@ -652,6 +646,12 @@
   </si>
   <si>
     <t>Código</t>
+  </si>
+  <si>
+    <t>Salada ee Frutas</t>
+  </si>
+  <si>
+    <t>Delicia de Uva</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D676422-48F4-486D-9387-1131E2D2335D}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,28 +1057,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1086,20 +1086,20 @@
         <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>42</v>
@@ -1110,11 +1110,11 @@
         <v>185</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>22</v>
@@ -1134,11 +1134,11 @@
         <v>150</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -1158,11 +1158,11 @@
         <v>149</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
@@ -1182,11 +1182,11 @@
         <v>151</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2">
@@ -1204,11 +1204,11 @@
         <v>186</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>22</v>
@@ -1228,13 +1228,13 @@
         <v>162</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>22</v>
@@ -1254,13 +1254,13 @@
         <v>180</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>2</v>
@@ -1280,11 +1280,11 @@
         <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>2</v>
@@ -1304,11 +1304,11 @@
         <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>2</v>
@@ -1328,11 +1328,11 @@
         <v>69</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>2</v>
@@ -1352,11 +1352,11 @@
         <v>67</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>2</v>
@@ -1376,11 +1376,11 @@
         <v>66</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
@@ -1400,11 +1400,11 @@
         <v>65</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>2</v>
@@ -1424,11 +1424,11 @@
         <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>2</v>
@@ -1448,11 +1448,11 @@
         <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>2</v>
@@ -1472,11 +1472,11 @@
         <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>2</v>
@@ -1496,11 +1496,11 @@
         <v>70</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>2</v>
@@ -1520,11 +1520,11 @@
         <v>68</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>2</v>
@@ -1544,11 +1544,11 @@
         <v>182</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>2</v>
@@ -1568,11 +1568,11 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>2</v>
@@ -1581,7 +1581,7 @@
         <v>8.5</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>42</v>
@@ -1592,20 +1592,20 @@
         <v>121</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>42</v>
@@ -1616,11 +1616,11 @@
         <v>143</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>2</v>
@@ -1629,7 +1629,7 @@
         <v>3.3</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>42</v>
@@ -1640,11 +1640,11 @@
         <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>2</v>
@@ -1653,7 +1653,7 @@
         <v>10.9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>42</v>
@@ -1664,11 +1664,11 @@
         <v>130</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>2</v>
@@ -1677,7 +1677,7 @@
         <v>12.9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>42</v>
@@ -1688,11 +1688,11 @@
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>2</v>
@@ -1701,7 +1701,7 @@
         <v>8.5</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>42</v>
@@ -1712,11 +1712,11 @@
         <v>90</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>2</v>
@@ -1736,11 +1736,11 @@
         <v>138</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>2</v>
@@ -1749,7 +1749,7 @@
         <v>9.9</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>42</v>
@@ -1760,13 +1760,13 @@
         <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>2</v>
@@ -1775,7 +1775,7 @@
         <v>7.9</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>42</v>
@@ -1786,13 +1786,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>2</v>
@@ -1801,7 +1801,7 @@
         <v>8.5</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>42</v>
@@ -1812,11 +1812,11 @@
         <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>2</v>
@@ -1836,11 +1836,11 @@
         <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>2</v>
@@ -1860,11 +1860,11 @@
         <v>137</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>2</v>
@@ -1873,7 +1873,7 @@
         <v>6.99</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>42</v>
@@ -1884,13 +1884,13 @@
         <v>184</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>2</v>
@@ -1910,13 +1910,13 @@
         <v>42</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>2</v>
@@ -1925,7 +1925,7 @@
         <v>8.5</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>42</v>
@@ -1936,11 +1936,11 @@
         <v>126</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>2</v>
@@ -1949,7 +1949,7 @@
         <v>10.9</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>42</v>
@@ -1960,20 +1960,20 @@
         <v>133</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>42</v>
@@ -1984,11 +1984,11 @@
         <v>84</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>2</v>
@@ -2008,11 +2008,11 @@
         <v>131</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>2</v>
@@ -2021,7 +2021,7 @@
         <v>12.5</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>42</v>
@@ -2032,13 +2032,13 @@
         <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>2</v>
@@ -2047,7 +2047,7 @@
         <v>8.5</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>42</v>
@@ -2058,13 +2058,13 @@
         <v>145</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>2</v>
@@ -2084,13 +2084,13 @@
         <v>147</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>2</v>
@@ -2110,11 +2110,11 @@
         <v>134</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>2</v>
@@ -2123,7 +2123,7 @@
         <v>7.9</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>42</v>
@@ -2134,11 +2134,11 @@
         <v>153</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>2</v>
@@ -2158,11 +2158,11 @@
         <v>152</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>22</v>
@@ -2182,11 +2182,11 @@
         <v>135</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>2</v>
@@ -2195,7 +2195,7 @@
         <v>7.9</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>42</v>
@@ -2206,13 +2206,13 @@
         <v>159</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>2</v>
@@ -2232,11 +2232,11 @@
         <v>154</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>2</v>
@@ -2256,13 +2256,13 @@
         <v>16</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>2</v>
@@ -2282,11 +2282,11 @@
         <v>136</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>2</v>
@@ -2295,7 +2295,7 @@
         <v>12.9</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>42</v>
@@ -2306,13 +2306,13 @@
         <v>167</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>2</v>
@@ -2332,13 +2332,13 @@
         <v>11</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>2</v>
@@ -2358,11 +2358,11 @@
         <v>155</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>2</v>
@@ -2382,13 +2382,13 @@
         <v>156</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>2</v>
@@ -2408,13 +2408,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>2</v>
@@ -2434,11 +2434,11 @@
         <v>15</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>2</v>
@@ -2458,11 +2458,11 @@
         <v>14</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>2</v>
@@ -2482,11 +2482,11 @@
         <v>13</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>2</v>
@@ -2506,13 +2506,13 @@
         <v>52</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>2</v>
@@ -2521,7 +2521,7 @@
         <v>8.5</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>42</v>
@@ -2532,11 +2532,11 @@
         <v>88</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>2</v>
@@ -2556,11 +2556,11 @@
         <v>74</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>2</v>
@@ -2580,11 +2580,11 @@
         <v>75</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>2</v>
@@ -2604,11 +2604,11 @@
         <v>89</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>2</v>
@@ -2628,22 +2628,22 @@
         <v>169</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F65" s="2">
         <v>15.9</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>42</v>
@@ -2654,13 +2654,13 @@
         <v>62</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>2</v>
@@ -2669,7 +2669,7 @@
         <v>8.5</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>42</v>
@@ -2680,7 +2680,7 @@
         <v>82</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">

</xml_diff>